<commit_message>
Updated CHE model - 2025-08-10 01:30
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/vt_vervestacks_CHE_v1.xlsx
+++ b/VerveStacks_CHE/vt_vervestacks_CHE_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C47AB9E-7563-4CCE-B635-2631E26C9A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09DFE4F4-8541-40E8-A7D0-0172FFAD47B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{2F8558DC-456A-409A-B723-82F6D1E3E94C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{F6EFE887-97C6-4022-96FA-BE0D6304CA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -499,79 +499,79 @@
     <t>annual</t>
   </si>
   <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_19_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_14_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_10_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_0_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_1_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_24_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_23_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_6_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_17_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_3_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_20_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_25_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_8_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_5_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_22_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_9_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_18_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_2_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_4_Missing Solar Capacity</t>
+  </si>
+  <si>
     <t>Aggregated Plant - IRENA Gap - CHE_11_Missing Solar Capacity</t>
   </si>
   <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_24_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_6_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_23_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_1_Missing Solar Capacity</t>
+    <t>Aggregated Plant - IRENA Gap - CHE_12_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_7_Missing Solar Capacity</t>
+  </si>
+  <si>
+    <t>Aggregated Plant - IRENA Gap - CHE_21_Missing Solar Capacity</t>
   </si>
   <si>
     <t>Aggregated Plant - IRENA Gap - CHE_13_Missing Solar Capacity</t>
   </si>
   <si>
     <t>Aggregated Plant - IRENA Gap - CHE_15_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_3_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_0_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_21_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_14_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_19_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_4_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_8_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_5_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_10_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_2_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_18_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_7_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_12_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_25_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_20_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_9_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_22_Missing Solar Capacity</t>
-  </si>
-  <si>
-    <t>Aggregated Plant - IRENA Gap - CHE_17_Missing Solar Capacity</t>
   </si>
   <si>
     <t>AF</t>
@@ -1147,7 +1147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE4849A-DE28-4426-A698-848B8DA2F2EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD3FD90-912E-4927-8E56-3EA2355BC56C}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -4133,7 +4133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C145F5F2-80E5-4928-9280-F3429FB3EB2B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D6A25A-639D-4B78-AF48-8A28184C8133}">
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4454,7 +4454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702C3353-2C10-47A4-BBE5-6CD12202D8C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB72638-7255-45D3-99B8-859F38EAAAA6}">
   <dimension ref="A1:T128"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9417,7 +9417,7 @@
         <v>2022</v>
       </c>
       <c r="E99" s="4">
-        <v>0.19782569372870323</v>
+        <v>0.16637932510042519</v>
       </c>
       <c r="F99" s="4">
         <v>1</v>
@@ -9449,7 +9449,7 @@
         <v>2022</v>
       </c>
       <c r="E100" s="3">
-        <v>0.16277902359433066</v>
+        <v>0.17279262926045061</v>
       </c>
       <c r="F100" s="3">
         <v>1</v>
@@ -9481,7 +9481,7 @@
         <v>2022</v>
       </c>
       <c r="E101" s="4">
-        <v>0.19828629679661561</v>
+        <v>0.16277902359433066</v>
       </c>
       <c r="F101" s="4">
         <v>1</v>
@@ -9513,7 +9513,7 @@
         <v>2022</v>
       </c>
       <c r="E102" s="3">
-        <v>0.16152827258311295</v>
+        <v>0.15291072157643879</v>
       </c>
       <c r="F102" s="3">
         <v>1</v>
@@ -9545,7 +9545,7 @@
         <v>2022</v>
       </c>
       <c r="E103" s="4">
-        <v>0.19328994063107527</v>
+        <v>0.16554834018408843</v>
       </c>
       <c r="F103" s="4">
         <v>1</v>
@@ -9577,7 +9577,7 @@
         <v>2022</v>
       </c>
       <c r="E104" s="3">
-        <v>0.21731537653220406</v>
+        <v>0.21471510601685545</v>
       </c>
       <c r="F104" s="3">
         <v>1</v>
@@ -9609,7 +9609,7 @@
         <v>2022</v>
       </c>
       <c r="E105" s="4">
-        <v>0.17279262926045061</v>
+        <v>0.15409499379434963</v>
       </c>
       <c r="F105" s="4">
         <v>1</v>
@@ -9641,7 +9641,7 @@
         <v>2022</v>
       </c>
       <c r="E106" s="3">
-        <v>0.15338177131187081</v>
+        <v>0.16152827258311295</v>
       </c>
       <c r="F106" s="3">
         <v>1</v>
@@ -9673,7 +9673,7 @@
         <v>2022</v>
       </c>
       <c r="E107" s="4">
-        <v>0.16637932510042519</v>
+        <v>0.13710016513395351</v>
       </c>
       <c r="F107" s="4">
         <v>1</v>
@@ -9705,7 +9705,7 @@
         <v>2022</v>
       </c>
       <c r="E108" s="3">
-        <v>0.16699472878703805</v>
+        <v>0.18308354646436523</v>
       </c>
       <c r="F108" s="3">
         <v>1</v>
@@ -9737,7 +9737,7 @@
         <v>2022</v>
       </c>
       <c r="E109" s="4">
-        <v>0.19614947844032105</v>
+        <v>0.15521278721895346</v>
       </c>
       <c r="F109" s="4">
         <v>1</v>
@@ -9769,7 +9769,7 @@
         <v>2022</v>
       </c>
       <c r="E110" s="3">
-        <v>0.17082200788742341</v>
+        <v>0.1586174511333161</v>
       </c>
       <c r="F110" s="3">
         <v>1</v>
@@ -9801,7 +9801,7 @@
         <v>2022</v>
       </c>
       <c r="E111" s="4">
-        <v>0.211523174241075</v>
+        <v>0.20091315882928704</v>
       </c>
       <c r="F111" s="4">
         <v>1</v>
@@ -9833,7 +9833,7 @@
         <v>2022</v>
       </c>
       <c r="E112" s="3">
-        <v>0.13606784444360143</v>
+        <v>0.1930981018275324</v>
       </c>
       <c r="F112" s="3">
         <v>1</v>
@@ -9865,7 +9865,7 @@
         <v>2022</v>
       </c>
       <c r="E113" s="4">
-        <v>0.18308354646436523</v>
+        <v>0.19782569372870323</v>
       </c>
       <c r="F113" s="4">
         <v>1</v>
@@ -9897,7 +9897,7 @@
         <v>2022</v>
       </c>
       <c r="E114" s="3">
-        <v>0.15291072157643879</v>
+        <v>0.16699472878703805</v>
       </c>
       <c r="F114" s="3">
         <v>1</v>
@@ -9929,7 +9929,7 @@
         <v>2022</v>
       </c>
       <c r="E115" s="4">
-        <v>0.16554834018408843</v>
+        <v>0.19614947844032105</v>
       </c>
       <c r="F115" s="4">
         <v>1</v>
@@ -9961,7 +9961,7 @@
         <v>2022</v>
       </c>
       <c r="E116" s="3">
-        <v>0.21471510601685545</v>
+        <v>0.17082200788742341</v>
       </c>
       <c r="F116" s="3">
         <v>1</v>
@@ -9993,7 +9993,7 @@
         <v>2022</v>
       </c>
       <c r="E117" s="4">
-        <v>0.15409499379434963</v>
+        <v>0.211523174241075</v>
       </c>
       <c r="F117" s="4">
         <v>1</v>
@@ -10025,7 +10025,7 @@
         <v>2022</v>
       </c>
       <c r="E118" s="3">
-        <v>0.13710016513395351</v>
+        <v>0.19328994063107527</v>
       </c>
       <c r="F118" s="3">
         <v>1</v>
@@ -10057,7 +10057,7 @@
         <v>2022</v>
       </c>
       <c r="E119" s="4">
-        <v>0.15521278721895346</v>
+        <v>0.21731537653220406</v>
       </c>
       <c r="F119" s="4">
         <v>1</v>
@@ -10089,7 +10089,7 @@
         <v>2022</v>
       </c>
       <c r="E120" s="3">
-        <v>0.1586174511333161</v>
+        <v>0.21077006448261207</v>
       </c>
       <c r="F120" s="3">
         <v>1</v>
@@ -10121,7 +10121,7 @@
         <v>2022</v>
       </c>
       <c r="E121" s="4">
-        <v>0.20091315882928704</v>
+        <v>0.19828629679661561</v>
       </c>
       <c r="F121" s="4">
         <v>1</v>
@@ -10153,7 +10153,7 @@
         <v>2022</v>
       </c>
       <c r="E122" s="3">
-        <v>0.1930981018275324</v>
+        <v>0.15338177131187081</v>
       </c>
       <c r="F122" s="3">
         <v>1</v>
@@ -10185,7 +10185,7 @@
         <v>2022</v>
       </c>
       <c r="E123" s="4">
-        <v>0.21077006448261207</v>
+        <v>0.13606784444360143</v>
       </c>
       <c r="F123" s="4">
         <v>1</v>

</xml_diff>